<commit_message>
Alteração nos artefatos de Garantia da Qualidade
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/7-Garantia da Qualidade/Templates/Registro de Auditorias.xlsx
+++ b/Artefatos de Documentação/Processo Genérico/7-Garantia da Qualidade/Templates/Registro de Auditorias.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Data de Abertura</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Executada</t>
+  </si>
+  <si>
+    <t>Planejada</t>
   </si>
 </sst>
 </file>
@@ -63,7 +66,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,6 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,8 +483,8 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="7" t="s">
-        <v>5</v>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -482,8 +492,8 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -491,8 +501,8 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -500,7 +510,9 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
@@ -521,14 +533,14 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
@@ -558,6 +570,9 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>